<commit_message>
update: instant_report & profile API
</commit_message>
<xml_diff>
--- a/data/0928Mock.xlsx
+++ b/data/0928Mock.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="166">
   <si>
     <t>题号</t>
   </si>
@@ -524,9 +524,6 @@
 D. 依赖他人安排 
 E. 经常拖延 
 F.没有时间观念</t>
-  </si>
-  <si>
-    <t>DEF</t>
   </si>
   <si>
     <t>{{appellation}}在和小伙伴相处时，更常见的表现是？</t>
@@ -1899,10 +1896,10 @@
   <sheetPr/>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" zoomScaleSheetLayoutView="60" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.3846153846154" defaultRowHeight="16.8"/>
@@ -1911,7 +1908,7 @@
     <col min="2" max="2" width="64.0961538461538" style="2" customWidth="1"/>
     <col min="3" max="4" width="52.5576923076923" style="2" customWidth="1"/>
     <col min="5" max="5" width="36.5288461538462" style="2" customWidth="1"/>
-    <col min="6" max="6" width="34.6057692307692" style="2" customWidth="1"/>
+    <col min="6" max="6" width="40.0576923076923" style="2" customWidth="1"/>
     <col min="7" max="7" width="30.6057692307692" style="2" customWidth="1"/>
     <col min="8" max="8" width="34.1346153846154" style="2" customWidth="1"/>
     <col min="9" max="9" width="31.7211538461538" style="2" customWidth="1"/>
@@ -3075,7 +3072,7 @@
         <v>14</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>118</v>
+        <v>48</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>14</v>
@@ -3104,10 +3101,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>14</v>
@@ -3142,10 +3139,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>14</v>
@@ -3180,10 +3177,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>14</v>
@@ -3218,10 +3215,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>14</v>
@@ -3256,10 +3253,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>14</v>
@@ -3294,10 +3291,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>14</v>
@@ -3332,10 +3329,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>14</v>
@@ -3370,10 +3367,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>14</v>
@@ -3408,10 +3405,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>14</v>
@@ -3446,10 +3443,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>14</v>
@@ -3484,10 +3481,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>14</v>
@@ -3522,10 +3519,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>14</v>
@@ -3560,10 +3557,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>14</v>
@@ -3598,10 +3595,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>14</v>
@@ -3636,10 +3633,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>14</v>
@@ -3674,10 +3671,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>14</v>
@@ -3712,10 +3709,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>14</v>
@@ -3733,7 +3730,7 @@
         <v>93</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>93</v>
@@ -3742,7 +3739,7 @@
         <v>93</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" ht="101" spans="1:12">
@@ -3750,37 +3747,37 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="J49" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="K49" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="L49" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="50" ht="101" spans="1:12">
@@ -3788,10 +3785,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>14</v>

</xml_diff>